<commit_message>
Pruebas con diferentes combinaciones de atributos y algoritmos
</commit_message>
<xml_diff>
--- a/src/Avistamientos/PruebasGeneracionModelo/Resultados Modelos.xlsx
+++ b/src/Avistamientos/PruebasGeneracionModelo/Resultados Modelos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\GitHub\Jellyfish_Forecast\src\Avistamientos\PruebasGeneracionModelo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94E2EFE6-3EC2-4D41-AC35-2C26DE579272}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90A79AD-3D57-4EF5-AE88-AE74C7DD04AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B48C8427-DF50-4C4A-A033-13916E0264EA}"/>
+    <workbookView xWindow="12420" yWindow="3645" windowWidth="21600" windowHeight="11835" xr2:uid="{B48C8427-DF50-4C4A-A033-13916E0264EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>Algoritmos</t>
   </si>
@@ -49,19 +49,177 @@
   </si>
   <si>
     <t>Arbol Decisión</t>
+  </si>
+  <si>
+    <t>0 dias</t>
+  </si>
+  <si>
+    <t>7 dias</t>
+  </si>
+  <si>
+    <t>14 dias</t>
+  </si>
+  <si>
+    <t>30 dias</t>
+  </si>
+  <si>
+    <t>45 dias</t>
+  </si>
+  <si>
+    <t>60 dias</t>
+  </si>
+  <si>
+    <t>0.09</t>
+  </si>
+  <si>
+    <t>0.26</t>
+  </si>
+  <si>
+    <t>Con SVC</t>
+  </si>
+  <si>
+    <t>{'max_depth': 81, 'max_features': 1, 'n_estimators': 183}</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.41</t>
+  </si>
+  <si>
+    <t>-0.03874</t>
+  </si>
+  <si>
+    <t>-0.196</t>
+  </si>
+  <si>
+    <t>0.059</t>
+  </si>
+  <si>
+    <t>0.155</t>
+  </si>
+  <si>
+    <t>0.07</t>
+  </si>
+  <si>
+    <t>0.28</t>
+  </si>
+  <si>
+    <t>-0.047</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>0.267</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>0.017</t>
+  </si>
+  <si>
+    <t>-0.060</t>
+  </si>
+  <si>
+    <t>-2.84</t>
+  </si>
+  <si>
+    <t>{'max_depth': 92, 'max_features': 1, 'n_estimators': 399}</t>
+  </si>
+  <si>
+    <t>-0.301</t>
+  </si>
+  <si>
+    <t>-0.44</t>
+  </si>
+  <si>
+    <t>-0.21</t>
+  </si>
+  <si>
+    <t>-0.98</t>
+  </si>
+  <si>
+    <t>-0.070</t>
+  </si>
+  <si>
+    <t>-1.56</t>
+  </si>
+  <si>
+    <t>0.110</t>
+  </si>
+  <si>
+    <t>0.17</t>
+  </si>
+  <si>
+    <t>{'max_depth': 30, 'max_features': 4, 'n_estimators': 36}</t>
+  </si>
+  <si>
+    <t>0.416</t>
+  </si>
+  <si>
+    <t>0.29</t>
+  </si>
+  <si>
+    <t>-0.136</t>
+  </si>
+  <si>
+    <t>0.1198</t>
+  </si>
+  <si>
+    <t>0.147</t>
+  </si>
+  <si>
+    <t>0.210</t>
+  </si>
+  <si>
+    <t>{'max_depth': 37, 'max_features': 1, 'n_estimators': 460}</t>
+  </si>
+  <si>
+    <t>0.344</t>
+  </si>
+  <si>
+    <t>-0.091</t>
+  </si>
+  <si>
+    <t>-1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 celdas </t>
+  </si>
+  <si>
+    <t>0 celda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,8 +242,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,48 +568,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E8B895-3058-473E-9C68-B29ACD60D5F3}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="4">
+        <v>-11605</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B4:G11">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:G4">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>